<commit_message>
Jan 2019 roll out
</commit_message>
<xml_diff>
--- a/docs/For-Portal-1Jan19.xlsx
+++ b/docs/For-Portal-1Jan19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trust-site\git\ceg94trust\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED550837-A161-4038-8916-C7CF2553A170}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B05D5A-C91E-4F42-B56E-E5A252042255}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="For Portal" sheetId="1" r:id="rId1"/>
@@ -1444,6 +1444,27 @@
     <xf numFmtId="168" fontId="7" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="17" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="18" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1477,27 +1498,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="17" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="18" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -2444,7 +2444,7 @@
                   <c:v>315524</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>323275</c:v>
+                  <c:v>309110</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>92938</c:v>
@@ -2550,6 +2550,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -7890,14 +7891,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>622934</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>137159</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>108584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>62865</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7975,6 +7976,136 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.66428</cdr:x>
+      <cdr:y>0.22614</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.46225</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C9402CF-5DE4-4978-897B-928A200C08B1}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="8007797" y="1036485"/>
+          <a:ext cx="2508308" cy="1082212"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="38100">
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="3200" b="1" dirty="0"/>
+            <a:t>22 Students</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="3200" b="1" dirty="0"/>
+            <a:t>₹7,17,572</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="3200" b="1" dirty="0">
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-IN" sz="3200" b="1" dirty="0"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8087,7 +8218,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -8374,7 +8505,7 @@
 </c:userShapes>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -9266,8 +9397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9278,7 +9409,7 @@
     <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="11.5546875"/>
     <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" customWidth="1"/>
     <col min="12" max="12" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.33203125" bestFit="1" customWidth="1"/>
@@ -9295,14 +9426,14 @@
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="126" t="s">
+      <c r="D3" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126" t="s">
+      <c r="E3" s="135"/>
+      <c r="F3" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="126"/>
+      <c r="G3" s="135"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
@@ -9346,14 +9477,14 @@
         <v>24250</v>
       </c>
       <c r="J5" s="31"/>
-      <c r="K5" s="127">
+      <c r="K5" s="136">
         <v>43282</v>
       </c>
-      <c r="L5" s="128"/>
-      <c r="M5" s="127">
+      <c r="L5" s="137"/>
+      <c r="M5" s="136">
         <v>43446</v>
       </c>
-      <c r="N5" s="128"/>
+      <c r="N5" s="137"/>
       <c r="O5" s="31"/>
     </row>
     <row r="6" spans="1:15" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
@@ -9473,8 +9604,7 @@
         <v>16</v>
       </c>
       <c r="K8" s="36">
-        <f t="shared" si="0"/>
-        <v>14165</v>
+        <v>0</v>
       </c>
       <c r="L8" s="36">
         <f t="shared" si="0"/>
@@ -9490,7 +9620,7 @@
       </c>
       <c r="O8" s="34">
         <f>SUM(K8:N8)</f>
-        <v>207195</v>
+        <v>193030</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
@@ -9618,7 +9748,7 @@
       </c>
       <c r="K11" s="40">
         <f>SUM(K7:K10)</f>
-        <v>14165</v>
+        <v>0</v>
       </c>
       <c r="L11" s="40">
         <f>SUM(L7:L10)</f>
@@ -9634,7 +9764,7 @@
       </c>
       <c r="O11" s="41">
         <f>SUM(K11:N11)</f>
-        <v>731737</v>
+        <v>717572</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="24.6" x14ac:dyDescent="0.4">
@@ -9666,7 +9796,7 @@
       <c r="L12" s="31"/>
       <c r="M12" s="55">
         <f>SUM(K11,M11)</f>
-        <v>160585</v>
+        <v>146420</v>
       </c>
       <c r="N12" s="31"/>
       <c r="O12" s="55">
@@ -9838,7 +9968,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="10">
-        <v>14165</v>
+        <v>0</v>
       </c>
       <c r="E18" s="10">
         <f>[1]Consolidated!G18</f>
@@ -10116,7 +10246,7 @@
       <c r="C27" s="13"/>
       <c r="D27" s="6">
         <f>SUM(D5:D26)</f>
-        <v>14165</v>
+        <v>0</v>
       </c>
       <c r="E27" s="6">
         <f>SUM(E5:E26)</f>
@@ -10145,7 +10275,7 @@
       </c>
       <c r="E28" s="15">
         <f>D27+E27</f>
-        <v>100826</v>
+        <v>86661</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>29</v>
@@ -10172,7 +10302,10 @@
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="19">
-        <f>[1]Consolidated!K35</f>
+        <f>E30-14165</f>
+        <v>309110</v>
+      </c>
+      <c r="E30" s="19">
         <v>323275</v>
       </c>
     </row>
@@ -10193,7 +10326,7 @@
       <c r="C32" s="20"/>
       <c r="D32" s="21">
         <f>SUM(D27:G27)</f>
-        <v>731737</v>
+        <v>717572</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="16"/>
@@ -10220,7 +10353,7 @@
       </c>
       <c r="D38" s="52">
         <f>D30</f>
-        <v>323275</v>
+        <v>309110</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
@@ -10243,7 +10376,7 @@
       </c>
       <c r="D40" s="30">
         <f>SUM(D37:D39)</f>
-        <v>731737</v>
+        <v>717572</v>
       </c>
     </row>
   </sheetData>
@@ -10290,14 +10423,14 @@
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="126" t="s">
+      <c r="D3" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126" t="s">
+      <c r="E3" s="135"/>
+      <c r="F3" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="126"/>
+      <c r="G3" s="135"/>
     </row>
     <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -10991,7 +11124,7 @@
   <dimension ref="A1:AMK24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G20" sqref="G20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11352,12 +11485,12 @@
       <c r="G16" s="90"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="130" t="s">
+      <c r="A17" s="139" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="130"/>
-      <c r="C17" s="130"/>
-      <c r="D17" s="130"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
       <c r="E17" s="92">
         <v>66894</v>
       </c>
@@ -11394,11 +11527,11 @@
       <c r="A19" s="90"/>
       <c r="B19" s="90"/>
       <c r="C19" s="91"/>
-      <c r="D19" s="130" t="s">
+      <c r="D19" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="130"/>
-      <c r="F19" s="130"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
       <c r="G19" s="92">
         <f>G20+G21</f>
         <v>717572</v>
@@ -11408,11 +11541,11 @@
       <c r="A20" s="90"/>
       <c r="B20" s="90"/>
       <c r="C20" s="91"/>
-      <c r="D20" s="131" t="s">
+      <c r="D20" s="140" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="132"/>
-      <c r="F20" s="133"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="142"/>
       <c r="G20" s="73">
         <f>315524</f>
         <v>315524</v>
@@ -11422,11 +11555,11 @@
       <c r="A21" s="90"/>
       <c r="B21" s="90"/>
       <c r="C21" s="91"/>
-      <c r="D21" s="134" t="s">
+      <c r="D21" s="143" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="135"/>
-      <c r="F21" s="136"/>
+      <c r="E21" s="144"/>
+      <c r="F21" s="145"/>
       <c r="G21" s="73">
         <v>402048</v>
       </c>
@@ -11435,11 +11568,11 @@
       <c r="A22" s="90"/>
       <c r="B22" s="90"/>
       <c r="C22" s="91"/>
-      <c r="D22" s="129" t="s">
+      <c r="D22" s="138" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
       <c r="G22" s="99">
         <f>F15+F17</f>
         <v>1717894</v>
@@ -11449,11 +11582,11 @@
       <c r="A23" s="90"/>
       <c r="B23" s="90"/>
       <c r="C23" s="91"/>
-      <c r="D23" s="129" t="s">
+      <c r="D23" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
+      <c r="E23" s="138"/>
+      <c r="F23" s="138"/>
       <c r="G23" s="99">
         <f>G15-G19</f>
         <v>572259</v>
@@ -11502,8 +11635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9706060-1731-41CB-8B93-05063862E976}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11533,7 +11666,7 @@
       <c r="F1" s="59"/>
       <c r="G1" s="60"/>
     </row>
-    <row r="2" spans="1:20" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="62" t="s">
         <v>52</v>
       </c>
@@ -11585,7 +11718,7 @@
       <c r="J3" s="123">
         <v>60000</v>
       </c>
-      <c r="K3" s="138">
+      <c r="K3" s="127">
         <f>$J3/$J$15</f>
         <v>2.0402396465488835E-2</v>
       </c>
@@ -11644,7 +11777,7 @@
         <f>N4+R4</f>
         <v>727450</v>
       </c>
-      <c r="K4" s="138">
+      <c r="K4" s="127">
         <f t="shared" ref="K4:K14" si="1">$J4/$J$15</f>
         <v>0.24736205514699758</v>
       </c>
@@ -11701,7 +11834,7 @@
       <c r="J5" s="123">
         <v>771916</v>
       </c>
-      <c r="K5" s="138">
+      <c r="K5" s="127">
         <f t="shared" si="1"/>
         <v>0.26248227116757133</v>
       </c>
@@ -11757,7 +11890,7 @@
       <c r="J6" s="123">
         <v>473280</v>
       </c>
-      <c r="K6" s="138">
+      <c r="K6" s="127">
         <f t="shared" si="1"/>
         <v>0.16093410331977595</v>
       </c>
@@ -11813,7 +11946,7 @@
       <c r="J7" s="123">
         <v>625003</v>
       </c>
-      <c r="K7" s="138">
+      <c r="K7" s="127">
         <f t="shared" si="1"/>
         <v>0.21252598330199865</v>
       </c>
@@ -11869,7 +12002,7 @@
       <c r="J8" s="123">
         <v>35000</v>
       </c>
-      <c r="K8" s="138">
+      <c r="K8" s="127">
         <f t="shared" si="1"/>
         <v>1.1901397938201821E-2</v>
       </c>
@@ -11925,7 +12058,7 @@
       <c r="J9" s="123">
         <v>55000</v>
       </c>
-      <c r="K9" s="138">
+      <c r="K9" s="127">
         <f t="shared" si="1"/>
         <v>1.8702196760031434E-2</v>
       </c>
@@ -11981,7 +12114,7 @@
       <c r="J10" s="123">
         <v>79307</v>
       </c>
-      <c r="K10" s="138">
+      <c r="K10" s="127">
         <f t="shared" si="1"/>
         <v>2.6967547608142052E-2</v>
       </c>
@@ -12037,7 +12170,7 @@
       <c r="J11" s="123">
         <v>20000</v>
       </c>
-      <c r="K11" s="138">
+      <c r="K11" s="127">
         <f t="shared" si="1"/>
         <v>6.8007988218296124E-3</v>
       </c>
@@ -12086,7 +12219,7 @@
       <c r="J12" s="124">
         <v>10000</v>
       </c>
-      <c r="K12" s="138">
+      <c r="K12" s="127">
         <f>$J12/$J$15</f>
         <v>3.4003994109148062E-3</v>
       </c>
@@ -12133,7 +12266,7 @@
       <c r="J13" s="124">
         <v>15000</v>
       </c>
-      <c r="K13" s="138">
+      <c r="K13" s="127">
         <f t="shared" si="1"/>
         <v>5.1005991163722087E-3</v>
       </c>
@@ -12183,7 +12316,7 @@
         <f>62875+6000</f>
         <v>68875</v>
       </c>
-      <c r="K14" s="138">
+      <c r="K14" s="127">
         <f t="shared" si="1"/>
         <v>2.3420250942675726E-2</v>
       </c>
@@ -12242,7 +12375,7 @@
         <f>SUM(J3:J14)</f>
         <v>2940831</v>
       </c>
-      <c r="K15" s="139">
+      <c r="K15" s="128">
         <f>SUM(K3:K14)</f>
         <v>1</v>
       </c>
@@ -12278,12 +12411,12 @@
       <c r="T16" s="103"/>
     </row>
     <row r="17" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="130" t="s">
+      <c r="A17" s="139" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="130"/>
-      <c r="C17" s="130"/>
-      <c r="D17" s="130"/>
+      <c r="B17" s="139"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
       <c r="E17" s="92">
         <v>66894</v>
       </c>
@@ -12318,11 +12451,11 @@
       <c r="A19" s="90"/>
       <c r="B19" s="90"/>
       <c r="C19" s="91"/>
-      <c r="D19" s="130" t="s">
+      <c r="D19" s="139" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="130"/>
-      <c r="F19" s="130"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
       <c r="G19" s="92">
         <f>G20+G21</f>
         <v>717572</v>
@@ -12332,11 +12465,11 @@
       <c r="A20" s="90"/>
       <c r="B20" s="90"/>
       <c r="C20" s="91"/>
-      <c r="D20" s="131" t="s">
+      <c r="D20" s="140" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="132"/>
-      <c r="F20" s="133"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="142"/>
       <c r="G20" s="73">
         <f>315524</f>
         <v>315524</v>
@@ -12346,18 +12479,18 @@
       <c r="A21" s="90"/>
       <c r="B21" s="90"/>
       <c r="C21" s="91"/>
-      <c r="D21" s="134" t="s">
+      <c r="D21" s="143" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="135"/>
-      <c r="F21" s="136"/>
+      <c r="E21" s="144"/>
+      <c r="F21" s="145"/>
       <c r="G21" s="73">
         <v>402048</v>
       </c>
       <c r="Q21" t="s">
         <v>86</v>
       </c>
-      <c r="R21" s="145">
+      <c r="R21" s="134">
         <f>E15</f>
         <v>2940831</v>
       </c>
@@ -12366,11 +12499,11 @@
       <c r="A22" s="90"/>
       <c r="B22" s="90"/>
       <c r="C22" s="91"/>
-      <c r="D22" s="129" t="s">
+      <c r="D22" s="138" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="138"/>
       <c r="G22" s="99">
         <f>F15+F17</f>
         <v>1717894</v>
@@ -12378,7 +12511,7 @@
       <c r="Q22" t="s">
         <v>90</v>
       </c>
-      <c r="R22" s="145">
+      <c r="R22" s="134">
         <f>G19</f>
         <v>717572</v>
       </c>
@@ -12387,11 +12520,11 @@
       <c r="A23" s="90"/>
       <c r="B23" s="90"/>
       <c r="C23" s="91"/>
-      <c r="D23" s="129" t="s">
+      <c r="D23" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="129"/>
-      <c r="F23" s="129"/>
+      <c r="E23" s="138"/>
+      <c r="F23" s="138"/>
       <c r="G23" s="99">
         <f>G15-G19</f>
         <v>572259</v>
@@ -12399,7 +12532,7 @@
       <c r="Q23" t="s">
         <v>88</v>
       </c>
-      <c r="R23" s="145">
+      <c r="R23" s="134">
         <f>G22</f>
         <v>1717894</v>
       </c>
@@ -12420,7 +12553,7 @@
       <c r="Q24" t="s">
         <v>87</v>
       </c>
-      <c r="R24" s="145">
+      <c r="R24" s="134">
         <f>F17</f>
         <v>66894</v>
       </c>
@@ -12429,7 +12562,7 @@
       <c r="Q25" t="s">
         <v>89</v>
       </c>
-      <c r="R25" s="145">
+      <c r="R25" s="134">
         <f>G23</f>
         <v>572259</v>
       </c>
@@ -12452,7 +12585,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D30" s="140" t="s">
+      <c r="D30" s="129" t="s">
         <v>76</v>
       </c>
       <c r="E30" s="118">
@@ -12470,7 +12603,7 @@
       </c>
     </row>
     <row r="31" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D31" s="140" t="s">
+      <c r="D31" s="129" t="s">
         <v>77</v>
       </c>
       <c r="E31" s="118">
@@ -12488,7 +12621,7 @@
       </c>
     </row>
     <row r="32" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D32" s="140" t="s">
+      <c r="D32" s="129" t="s">
         <v>78</v>
       </c>
       <c r="E32" s="118">
@@ -12506,7 +12639,7 @@
       </c>
     </row>
     <row r="33" spans="4:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D33" s="140" t="s">
+      <c r="D33" s="129" t="s">
         <v>79</v>
       </c>
       <c r="E33" s="118">
@@ -12522,7 +12655,7 @@
       </c>
     </row>
     <row r="34" spans="4:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="D34" s="141" t="s">
+      <c r="D34" s="130" t="s">
         <v>80</v>
       </c>
       <c r="E34" s="118">
@@ -12536,7 +12669,7 @@
         <f>I35/1000</f>
         <v>0</v>
       </c>
-      <c r="I34" s="137">
+      <c r="I34" s="126">
         <f>SUM(J34:J36)</f>
         <v>93875</v>
       </c>
@@ -12551,7 +12684,7 @@
         <f>I36/1000</f>
         <v>0</v>
       </c>
-      <c r="I35" s="137"/>
+      <c r="I35" s="126"/>
       <c r="J35" s="124">
         <v>15000</v>
       </c>
@@ -12564,7 +12697,7 @@
         <f>I34/1000</f>
         <v>93.875</v>
       </c>
-      <c r="I36" s="137"/>
+      <c r="I36" s="126"/>
       <c r="J36" s="124">
         <f>62875+6000</f>
         <v>68875</v>
@@ -12574,65 +12707,65 @@
       <c r="I37" s="93"/>
     </row>
     <row r="38" spans="4:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D38" s="140" t="s">
+      <c r="D38" s="129" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="142">
+      <c r="E38" s="131">
         <f>459000-6000</f>
         <v>453000</v>
       </c>
-      <c r="F38" s="143">
+      <c r="F38" s="132">
         <v>274450</v>
       </c>
-      <c r="G38" s="137">
+      <c r="G38" s="126">
         <f>N4+R4</f>
         <v>727450</v>
       </c>
     </row>
     <row r="39" spans="4:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D39" s="140" t="s">
+      <c r="D39" s="129" t="s">
         <v>82</v>
       </c>
-      <c r="E39" s="142">
+      <c r="E39" s="131">
         <v>498000</v>
       </c>
-      <c r="F39" s="143">
+      <c r="F39" s="132">
         <v>273916</v>
       </c>
-      <c r="G39" s="137">
+      <c r="G39" s="126">
         <v>771916</v>
       </c>
     </row>
     <row r="40" spans="4:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D40" s="140" t="s">
+      <c r="D40" s="129" t="s">
         <v>83</v>
       </c>
-      <c r="E40" s="142">
+      <c r="E40" s="131">
         <v>210000</v>
       </c>
-      <c r="F40" s="143">
+      <c r="F40" s="132">
         <v>263280</v>
       </c>
-      <c r="G40" s="137">
+      <c r="G40" s="126">
         <v>473280</v>
       </c>
     </row>
     <row r="41" spans="4:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D41" s="140" t="s">
+      <c r="D41" s="129" t="s">
         <v>84</v>
       </c>
-      <c r="E41" s="142">
+      <c r="E41" s="131">
         <v>285000</v>
       </c>
-      <c r="F41" s="143">
+      <c r="F41" s="132">
         <v>340003</v>
       </c>
-      <c r="G41" s="137">
+      <c r="G41" s="126">
         <v>625003</v>
       </c>
     </row>
     <row r="42" spans="4:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D42" s="144" t="s">
+      <c r="D42" s="133" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>